<commit_message>
Save my current changes before pulling
</commit_message>
<xml_diff>
--- a/gemini_output.xlsx
+++ b/gemini_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,512 +483,135 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>INGRAM MICRO ASIA PTE LTD</t>
+          <t>3D Trading Pte Ltd</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-02-24</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>MICROSOFT 365 BUS STD ESD 1 YEAR SUBSCRI</t>
+          <t>CASIO GEN</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E2" t="n">
-        <v>150</v>
+        <v>12</v>
       </c>
       <c r="F2" t="n">
-        <v>150</v>
-      </c>
-      <c r="G2" t="n">
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="H2" t="n">
-        <v>13.5</v>
+        <v>4.95</v>
       </c>
       <c r="I2" t="n">
-        <v>163.5</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>GAIN CITY BEST-ELECTRIC PTE LTD</t>
+          <t>AZ Gift &amp; Trading</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-02-22</t>
+          <t>2025-02-13</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>SONY WI-C100N WIRLESS EARPHONE - BLACK WI-C100N/BCE</t>
+          <t>Light Stick [6"]</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E3" t="n">
-        <v>40</v>
+        <v>1.5</v>
       </c>
       <c r="F3" t="n">
-        <v>30</v>
+        <v>22.5</v>
       </c>
       <c r="G3" t="n">
-        <v>27.52</v>
+        <v>20.64</v>
       </c>
       <c r="H3" t="n">
-        <v>2.48</v>
+        <v>1.86</v>
       </c>
       <c r="I3" t="n">
-        <v>30</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Challenger</t>
+          <t>HORME HARDWARE PTE LTD</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-02-13</t>
+          <t>2025-02-10</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Xiaomi Redmi A3 4+128GB Midnight Black LTE</t>
+          <t>[312646916-1L] NIPPON MULTI-SURFACE PRIMER (ONLY FOR WA TER BASE PAINT) 1L</t>
         </is>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>129</v>
+        <v>25</v>
       </c>
       <c r="F4" t="n">
-        <v>129</v>
-      </c>
-      <c r="G4" t="n">
-        <v>258</v>
+        <v>25</v>
       </c>
       <c r="H4" t="n">
-        <v>21.3</v>
+        <v>2.06</v>
       </c>
       <c r="I4" t="n">
-        <v>258</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Challenger</t>
+          <t>Amazon EU S.à r.l., UK Branch</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-02-13</t>
+          <t>2025-02-15</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Xiaomi Redmi A3 4+128GB Midnight Black LTE</t>
+          <t>Brother TN-243BK/TN-243C/TN-243M/TN-243Y Toner Cartridges, Black/Cyan/Magenta/Yellow, Multi-Pack, Standard Yield, Includes 4 x Toner Cartridges, Brother Genuine Supplies | B07FXXKFSC</t>
         </is>
       </c>
       <c r="D5" t="n">
         <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>129</v>
+        <v>128.19</v>
       </c>
       <c r="F5" t="n">
-        <v>129</v>
+        <v>139.73</v>
       </c>
       <c r="G5" t="n">
-        <v>258</v>
+        <v>161.96</v>
       </c>
       <c r="H5" t="n">
-        <v>21.3</v>
+        <v>14.58</v>
       </c>
       <c r="I5" t="n">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>3D Trading Pte Ltd</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2025-02-24</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>CASIO GEN</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>5</v>
-      </c>
-      <c r="E6" t="n">
-        <v>12</v>
-      </c>
-      <c r="F6" t="n">
-        <v>60</v>
-      </c>
-      <c r="H6" t="n">
-        <v>4.95</v>
-      </c>
-      <c r="I6" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>AZ Gift &amp; Trading</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2025-02-13</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Light Stick [6"]</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>15</v>
-      </c>
-      <c r="E7" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="F7" t="n">
-        <v>22.5</v>
-      </c>
-      <c r="G7" t="n">
-        <v>20.64</v>
-      </c>
-      <c r="H7" t="n">
-        <v>1.86</v>
-      </c>
-      <c r="I7" t="n">
-        <v>22.5</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Amazon EU S.à r.l., UK Branch</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2025-02-15</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Brother TN-243BK/TN-243C/TN-243M/TN-243Y Toner Cartridges, Black/Cyan/Magenta/Yellow, Multi-Pack, Standard Yield, Includes 4 x Toner Cartridges, Brother Genuine Supplies | B07FXXKFSC</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" t="n">
-        <v>128.19</v>
-      </c>
-      <c r="F8" t="n">
-        <v>139.73</v>
-      </c>
-      <c r="G8" t="n">
-        <v>161.96</v>
-      </c>
-      <c r="H8" t="n">
-        <v>14.58</v>
-      </c>
-      <c r="I8" t="n">
         <v>176.54</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Amazon EU S.à r.l., UK Branch</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>2025-02-15</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Shipping Charges</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" t="n">
-        <v>33.77</v>
-      </c>
-      <c r="F9" t="n">
-        <v>36.81</v>
-      </c>
-      <c r="G9" t="n">
-        <v>161.96</v>
-      </c>
-      <c r="H9" t="n">
-        <v>14.58</v>
-      </c>
-      <c r="I9" t="n">
-        <v>176.54</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>amazon.co.uk</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>2025-02-15</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Brother TN-243BK/TN-243C/TN-243M/TN-243Y Toner Cartridges, Black/Cyan/Magenta/Yellow, Multi-Pack, Standard Yield, Includes 4 x Toner Cartridges, Brother Genuine Supplies | B07FXXKFSC</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E10" t="n">
-        <v>128.19</v>
-      </c>
-      <c r="F10" t="n">
-        <v>139.73</v>
-      </c>
-      <c r="G10" t="n">
-        <v>161.96</v>
-      </c>
-      <c r="H10" t="n">
-        <v>14.58</v>
-      </c>
-      <c r="I10" t="n">
-        <v>176.54</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>amazon.co.uk</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>2025-02-15</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Shipping Charges</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>1</v>
-      </c>
-      <c r="E11" t="n">
-        <v>33.77</v>
-      </c>
-      <c r="F11" t="n">
-        <v>36.81</v>
-      </c>
-      <c r="G11" t="n">
-        <v>161.96</v>
-      </c>
-      <c r="H11" t="n">
-        <v>14.58</v>
-      </c>
-      <c r="I11" t="n">
-        <v>176.54</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Amazon EU S.à r.l., UK Branch</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>2025-02-15</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Brother TN-243BK/TN-243C/TN-243M/TN-243Y Toner Cartridges, Black/Cyan/Magenta/Yellow, Multi-Pack, Standard Yield, Includes 4 x Toner Cartridges, Brother Genuine Supplies | B07FXXKFSC</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>1</v>
-      </c>
-      <c r="E12" t="n">
-        <v>128.19</v>
-      </c>
-      <c r="F12" t="n">
-        <v>139.73</v>
-      </c>
-      <c r="G12" t="n">
-        <v>161.96</v>
-      </c>
-      <c r="H12" t="n">
-        <v>14.58</v>
-      </c>
-      <c r="I12" t="n">
-        <v>176.54</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>3D Trading Pte Ltd</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>2025-02-24</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>CASIO GEN</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>5</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>12.00</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>60.00</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>4.95</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>60.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>AZ Gift &amp; Trading</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>2025-02-13</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Light Stick [6"]</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>15</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>1.50</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>22.50</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>20.64</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>1.86</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>22.50</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>HORME HARDWARE PTE LTD</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>2025-02-10</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>[312646916-1L] NIPPON MULTI-SURFACE PRIMER (ONLY FOR WA TER BASE PAINT) 1L</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>25.00</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>25.00</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>2.06</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>25.00</t>
-        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>